<commit_message>
Prepare release 2.0.0 (#42)
* prepare release

* update release notes

* update release notes c27419a4d29cdcec7144c6479f1dcb9767e45a8b
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-cds-fr-related-person.xlsx
+++ b/main/ig/StructureDefinition-cds-fr-related-person.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0-ballot</t>
+    <t>2.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -51,7 +51,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-07-04T12:00:42+00:00</t>
+    <t>2024-09-24T12:46:07+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>